<commit_message>
may 2025 review 2
</commit_message>
<xml_diff>
--- a/carcass_2025_may.xlsx
+++ b/carcass_2025_may.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\pesquisa-bio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB706EC1-B360-4D86-A375-C4F3D55BCBDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A42F55CE-2A69-48DA-9A28-C077570AD9A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{BFCAABBE-2970-4592-9844-6A85260AFB1F}"/>
+    <workbookView xWindow="57480" yWindow="15945" windowWidth="29040" windowHeight="15720" xr2:uid="{BFCAABBE-2970-4592-9844-6A85260AFB1F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="52">
   <si>
     <t>Amostra</t>
   </si>
@@ -189,6 +189,9 @@
   </si>
   <si>
     <t>D8-4</t>
+  </si>
+  <si>
+    <t>A8-4</t>
   </si>
 </sst>
 </file>
@@ -327,34 +330,6 @@
   <dxfs count="7">
     <dxf>
       <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -475,19 +450,47 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
       </border>
     </dxf>
     <dxf>
-      <border outline="0">
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color auto="1"/>
         </left>
-        <top style="thin">
+        <right style="thin">
           <color auto="1"/>
-        </top>
+        </right>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
   </dxfs>
@@ -504,13 +507,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AB7B23FB-65CD-4981-9209-F2A38126FA9B}" name="Table1" displayName="Table1" ref="A1:D97" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="5" tableBorderDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AB7B23FB-65CD-4981-9209-F2A38126FA9B}" name="Table1" displayName="Table1" ref="A1:D97" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4">
   <autoFilter ref="A1:D97" xr:uid="{AB7B23FB-65CD-4981-9209-F2A38126FA9B}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{4745B1F8-33AB-40D6-A7C6-FACA34ACA0F6}" name="Amostra" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{182E2021-EA0B-407C-A2FD-D24E9A4B55EB}" name="RPL32" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{F7989474-8EE4-403F-9F26-000F912F561D}" name="VGR " dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{EC1CD5C4-EB92-49CF-A106-5D0D02DD51E6}" name="VG " dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{4745B1F8-33AB-40D6-A7C6-FACA34ACA0F6}" name="Amostra" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{182E2021-EA0B-407C-A2FD-D24E9A4B55EB}" name="RPL32" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{F7989474-8EE4-403F-9F26-000F912F561D}" name="VGR " dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{EC1CD5C4-EB92-49CF-A106-5D0D02DD51E6}" name="VG " dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -815,8 +818,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD8EA3E1-06F4-4028-8BC1-1F7D25846EBF}">
   <dimension ref="A1:D97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection sqref="A1:D97"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1149,7 +1152,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
-        <v>10</v>
+        <v>51</v>
       </c>
       <c r="B24" s="2">
         <v>17.340248784743309</v>
@@ -1163,7 +1166,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
-        <v>10</v>
+        <v>51</v>
       </c>
       <c r="B25" s="2">
         <v>17.875309195726388</v>

</xml_diff>